<commit_message>
alertas y correciones generales
</commit_message>
<xml_diff>
--- a/registros_excel/2024-01-29.xlsx
+++ b/registros_excel/2024-01-29.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,6 +588,191 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>101546</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Operaciones</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>11:9:21</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>11:09:22</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>11:09:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>101546</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Operaciones</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>11:13:37</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>11:09:22</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>11:13:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Adm</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Operaciones</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>13:6:27</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10:54:04</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>13:06:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>15961357</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mauricio Sanchez</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>13:6:30</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>10:54:06</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>13:06:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1054398414</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Julian Largo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>13:6:31</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10:54:08</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13:06:31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>